<commit_message>
Added bar codes to D5
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSM_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSM_00002.xlsx
@@ -20,12 +20,12 @@
     <sheet name="ACS182_CC_tcarray" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="210">
   <si>
     <t>Ref Des</t>
   </si>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:AMM220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34672,6 +34672,7 @@
       <c r="H34" s="16" t="s">
         <v>51</v>
       </c>
+      <c r="K34"/>
     </row>
     <row r="35" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A35"/>
@@ -34683,6 +34684,7 @@
       <c r="G35" s="14"/>
       <c r="H35"/>
       <c r="I35"/>
+      <c r="K35"/>
     </row>
     <row r="36" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
@@ -34710,6 +34712,7 @@
         <v>53</v>
       </c>
       <c r="I36"/>
+      <c r="K36"/>
     </row>
     <row r="37" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
@@ -34737,6 +34740,7 @@
         <v>54</v>
       </c>
       <c r="I37"/>
+      <c r="K37"/>
     </row>
     <row r="38" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -34764,6 +34768,7 @@
         <v>22.7</v>
       </c>
       <c r="I38"/>
+      <c r="K38"/>
     </row>
     <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
@@ -34791,6 +34796,7 @@
         <v>55</v>
       </c>
       <c r="I39"/>
+      <c r="K39"/>
     </row>
     <row r="40" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -34818,6 +34824,7 @@
         <v>56</v>
       </c>
       <c r="I40"/>
+      <c r="K40"/>
     </row>
     <row r="41" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
@@ -34845,6 +34852,7 @@
         <v>57</v>
       </c>
       <c r="I41"/>
+      <c r="K41"/>
     </row>
     <row r="42" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
@@ -34872,6 +34880,7 @@
         <v>58</v>
       </c>
       <c r="I42"/>
+      <c r="K42"/>
     </row>
     <row r="43" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
@@ -34900,6 +34909,7 @@
       </c>
       <c r="I43"/>
       <c r="J43"/>
+      <c r="K43"/>
     </row>
     <row r="44" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A44"/>
@@ -34911,14 +34921,13 @@
       <c r="G44" s="14"/>
       <c r="H44"/>
       <c r="I44"/>
+      <c r="K44"/>
     </row>
     <row r="45" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="J45" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K45" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K45"/>
       <c r="L45" s="12">
         <v>2</v>
       </c>
@@ -34937,9 +34946,7 @@
       <c r="J46" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K46" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K46"/>
       <c r="L46" s="12">
         <v>2</v>
       </c>
@@ -34958,9 +34965,7 @@
       <c r="J47" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K47" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K47"/>
       <c r="L47" s="12">
         <v>2</v>
       </c>
@@ -34979,9 +34984,7 @@
       <c r="J48" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K48" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K48"/>
       <c r="L48" s="12">
         <v>2</v>
       </c>
@@ -35000,9 +35003,7 @@
       <c r="J49" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K49" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K49"/>
       <c r="L49" s="12">
         <v>2</v>
       </c>
@@ -35021,9 +35022,7 @@
       <c r="J50" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K50" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K50"/>
       <c r="L50" s="12">
         <v>2</v>
       </c>
@@ -35042,9 +35041,7 @@
       <c r="J51" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K51" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K51"/>
       <c r="L51" s="12">
         <v>2</v>
       </c>
@@ -35065,9 +35062,7 @@
       <c r="J52" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K52" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K52"/>
       <c r="L52" s="12">
         <v>2</v>
       </c>
@@ -35088,9 +35083,7 @@
       <c r="J53" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K53" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K53"/>
       <c r="L53" s="12">
         <v>2</v>
       </c>
@@ -35111,9 +35104,7 @@
       <c r="J54" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K54" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K54"/>
       <c r="L54" s="12">
         <v>2</v>
       </c>
@@ -35140,6 +35131,7 @@
       <c r="G55" s="14"/>
       <c r="H55"/>
       <c r="I55"/>
+      <c r="K55"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -35167,6 +35159,7 @@
         <v>49</v>
       </c>
       <c r="I56"/>
+      <c r="K56"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
@@ -35194,6 +35187,7 @@
         <v>1.8369999999999999E-6</v>
       </c>
       <c r="I57"/>
+      <c r="K57"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
@@ -35221,6 +35215,7 @@
         <v>50</v>
       </c>
       <c r="I58"/>
+      <c r="K58"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
@@ -35248,6 +35243,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="I59"/>
+      <c r="K59"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
@@ -35275,6 +35271,7 @@
         <v>43</v>
       </c>
       <c r="I60"/>
+      <c r="K60"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
@@ -35302,6 +35299,7 @@
         <v>8.9599999999999999E-2</v>
       </c>
       <c r="I61"/>
+      <c r="K61"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
@@ -35331,6 +35329,7 @@
       <c r="I62" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K62"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
@@ -35360,6 +35359,7 @@
       <c r="I63" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K63"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
@@ -35389,6 +35389,7 @@
       <c r="I64" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K64"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
@@ -35418,6 +35419,7 @@
       <c r="I65" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K65"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66"/>
@@ -35429,14 +35431,13 @@
       <c r="G66" s="14"/>
       <c r="H66"/>
       <c r="I66"/>
+      <c r="K66"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J67" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K67" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K67"/>
       <c r="L67" s="12">
         <v>2</v>
       </c>
@@ -35454,9 +35455,7 @@
       <c r="J68" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K68" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K68"/>
       <c r="L68" s="12">
         <v>2</v>
       </c>
@@ -35474,9 +35473,7 @@
       <c r="J69" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K69" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K69"/>
       <c r="L69" s="12">
         <v>2</v>
       </c>
@@ -35494,9 +35491,7 @@
       <c r="J70" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K70" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K70"/>
       <c r="L70" s="12">
         <v>2</v>
       </c>
@@ -35514,9 +35509,7 @@
       <c r="J71" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K71" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K71"/>
       <c r="L71" s="12">
         <v>2</v>
       </c>
@@ -35534,9 +35527,7 @@
       <c r="J72" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K72" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K72"/>
       <c r="L72" s="12">
         <v>2</v>
       </c>
@@ -35554,9 +35545,7 @@
       <c r="J73" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K73" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K73"/>
       <c r="L73" s="12">
         <v>2</v>
       </c>
@@ -35574,9 +35563,7 @@
       <c r="J74" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K74" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K74"/>
       <c r="L74" s="12">
         <v>2</v>
       </c>
@@ -35594,9 +35581,7 @@
       <c r="J75" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K75" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K75"/>
       <c r="L75" s="12">
         <v>2</v>
       </c>
@@ -35614,9 +35599,7 @@
       <c r="J76" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K76" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K76"/>
       <c r="L76" s="12">
         <v>2</v>
       </c>
@@ -35634,9 +35617,7 @@
       <c r="J77" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K77" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K77"/>
       <c r="L77" s="12">
         <v>2</v>
       </c>
@@ -35654,9 +35635,7 @@
       <c r="J78" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K78" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K78"/>
       <c r="L78" s="12">
         <v>2</v>
       </c>
@@ -35674,9 +35653,7 @@
       <c r="J79" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K79" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K79"/>
       <c r="L79" s="12">
         <v>2</v>
       </c>
@@ -35694,9 +35671,7 @@
       <c r="J80" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K80" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K80"/>
       <c r="L80" s="12">
         <v>2</v>
       </c>
@@ -35714,9 +35689,7 @@
       <c r="J81" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K81" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K81"/>
       <c r="L81" s="12">
         <v>2</v>
       </c>
@@ -35734,9 +35707,7 @@
       <c r="J82" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K82" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K82"/>
       <c r="L82" s="12">
         <v>2</v>
       </c>
@@ -35754,9 +35725,7 @@
       <c r="J83" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K83" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K83"/>
       <c r="L83" s="12">
         <v>2</v>
       </c>
@@ -35774,9 +35743,7 @@
       <c r="J84" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K84" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K84"/>
       <c r="L84" s="12">
         <v>2</v>
       </c>
@@ -35794,9 +35761,7 @@
       <c r="J85" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K85" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K85"/>
       <c r="L85" s="12">
         <v>2</v>
       </c>
@@ -35814,9 +35779,7 @@
       <c r="J86" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K86" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K86"/>
       <c r="L86" s="12">
         <v>2</v>
       </c>
@@ -35834,9 +35797,7 @@
       <c r="J87" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K87" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K87"/>
       <c r="L87" s="12">
         <v>2</v>
       </c>
@@ -35854,9 +35815,7 @@
       <c r="J88" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K88" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K88"/>
       <c r="L88" s="12">
         <v>2</v>
       </c>
@@ -35874,9 +35833,7 @@
       <c r="J89" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K89" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K89"/>
       <c r="L89" s="12">
         <v>2</v>
       </c>
@@ -35894,9 +35851,7 @@
       <c r="J90" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K90" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="K90"/>
       <c r="L90" s="12">
         <v>2</v>
       </c>
@@ -35920,6 +35875,7 @@
       <c r="G91" s="14"/>
       <c r="H91"/>
       <c r="I91"/>
+      <c r="K91"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
@@ -35947,6 +35903,7 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I92"/>
+      <c r="K92"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
@@ -35974,6 +35931,7 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I93"/>
+      <c r="K93"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
@@ -36002,6 +35960,7 @@
       </c>
       <c r="I94"/>
       <c r="J94"/>
+      <c r="K94"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
@@ -36030,6 +35989,7 @@
       </c>
       <c r="I95"/>
       <c r="J95"/>
+      <c r="K95"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
@@ -36057,8 +36017,9 @@
         <v>-1.164927E-6</v>
       </c>
       <c r="I96"/>
+      <c r="K96"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>73</v>
       </c>
@@ -36084,8 +36045,9 @@
         <v>1.828527E-7</v>
       </c>
       <c r="I97"/>
+      <c r="K97"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>73</v>
       </c>
@@ -36111,8 +36073,9 @@
         <v>-60.958993499999998</v>
       </c>
       <c r="I98"/>
+      <c r="K98"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>73</v>
       </c>
@@ -36138,8 +36101,9 @@
         <v>54.631500299999999</v>
       </c>
       <c r="I99"/>
+      <c r="K99"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>73</v>
       </c>
@@ -36165,8 +36129,9 @@
         <v>-0.80724953099999996</v>
       </c>
       <c r="I100"/>
+      <c r="K100"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>73</v>
       </c>
@@ -36192,8 +36157,9 @@
         <v>524737.08900000004</v>
       </c>
       <c r="I101"/>
+      <c r="K101"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>73</v>
       </c>
@@ -36219,8 +36185,9 @@
         <v>17.629218300000002</v>
       </c>
       <c r="I102"/>
+      <c r="K102"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>73</v>
       </c>
@@ -36246,8 +36213,9 @@
         <v>-0.43791688400000001</v>
       </c>
       <c r="I103"/>
+      <c r="K103"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>73</v>
       </c>
@@ -36273,8 +36241,9 @@
         <v>25.067125000000001</v>
       </c>
       <c r="I104"/>
+      <c r="K104"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>73</v>
       </c>
@@ -36300,8 +36269,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="I105"/>
+      <c r="K105"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>73</v>
       </c>
@@ -36327,8 +36297,9 @@
         <v>0</v>
       </c>
       <c r="I106"/>
+      <c r="K106"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>73</v>
       </c>
@@ -36354,8 +36325,9 @@
         <v>8.5999905299999999E-2</v>
       </c>
       <c r="I107"/>
+      <c r="K107"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>73</v>
       </c>
@@ -36381,8 +36353,9 @@
         <v>4.8842670400000004E-4</v>
       </c>
       <c r="I108"/>
+      <c r="K108"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>73</v>
       </c>
@@ -36408,8 +36381,9 @@
         <v>-6.8426125900000003E-12</v>
       </c>
       <c r="I109"/>
+      <c r="K109"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>73</v>
       </c>
@@ -36435,8 +36409,9 @@
         <v>-0.99330379999999996</v>
       </c>
       <c r="I110"/>
+      <c r="K110"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>73</v>
       </c>
@@ -36462,8 +36437,9 @@
         <v>0.13849600000000001</v>
       </c>
       <c r="I111"/>
+      <c r="K111"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>73</v>
       </c>
@@ -36489,8 +36465,9 @@
         <v>-2.270537E-4</v>
       </c>
       <c r="I112"/>
+      <c r="K112"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>73</v>
       </c>
@@ -36516,8 +36493,9 @@
         <v>3.540078E-5</v>
       </c>
       <c r="I113"/>
+      <c r="K113"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>73</v>
       </c>
@@ -36543,8 +36521,9 @@
         <v>-9.5700000000000003E-8</v>
       </c>
       <c r="I114"/>
+      <c r="K114"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>73</v>
       </c>
@@ -36570,8 +36549,9 @@
         <v>3.2499999999999998E-6</v>
       </c>
       <c r="I115"/>
+      <c r="K115"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -36581,8 +36561,9 @@
       <c r="G116" s="14"/>
       <c r="H116"/>
       <c r="I116"/>
+      <c r="K116"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>96</v>
       </c>
@@ -36608,8 +36589,9 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I117"/>
+      <c r="K117"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>96</v>
       </c>
@@ -36635,8 +36617,9 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I118"/>
+      <c r="K118"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>96</v>
       </c>
@@ -36662,8 +36645,9 @@
         <v>1.2589159999999999E-3</v>
       </c>
       <c r="I119"/>
+      <c r="K119"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>96</v>
       </c>
@@ -36689,8 +36673,9 @@
         <v>2.7384590000000003E-4</v>
       </c>
       <c r="I120"/>
+      <c r="K120"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>96</v>
       </c>
@@ -36716,8 +36701,9 @@
         <v>-1.1230929999999999E-6</v>
       </c>
       <c r="I121"/>
+      <c r="K121"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>96</v>
       </c>
@@ -36743,8 +36729,9 @@
         <v>1.8295270000000001E-7</v>
       </c>
       <c r="I122"/>
+      <c r="K122"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>96</v>
       </c>
@@ -36770,8 +36757,9 @@
         <v>-58.694972800000002</v>
       </c>
       <c r="I123"/>
+      <c r="K123"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>96</v>
       </c>
@@ -36797,8 +36785,9 @@
         <v>54.6728393</v>
       </c>
       <c r="I124"/>
+      <c r="K124"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>96</v>
       </c>
@@ -36824,8 +36813,9 @@
         <v>-0.63763615600000001</v>
       </c>
       <c r="I125"/>
+      <c r="K125"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>96</v>
       </c>
@@ -36851,8 +36841,9 @@
         <v>524643.36600000004</v>
       </c>
       <c r="I126"/>
+      <c r="K126"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>96</v>
       </c>
@@ -36878,8 +36869,9 @@
         <v>24.075237300000001</v>
       </c>
       <c r="I127"/>
+      <c r="K127"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>96</v>
       </c>
@@ -36906,8 +36898,9 @@
       </c>
       <c r="I128"/>
       <c r="J128"/>
+      <c r="K128"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>96</v>
       </c>
@@ -36933,8 +36926,9 @@
         <v>25.027625</v>
       </c>
       <c r="I129"/>
+      <c r="K129"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
         <v>96</v>
       </c>
@@ -36961,8 +36955,9 @@
       </c>
       <c r="I130"/>
       <c r="J130"/>
+      <c r="K130"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>96</v>
       </c>
@@ -36988,8 +36983,9 @@
         <v>0</v>
       </c>
       <c r="I131"/>
+      <c r="K131"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>96</v>
       </c>
@@ -37015,8 +37011,9 @@
         <v>0.120444996</v>
       </c>
       <c r="I132"/>
+      <c r="K132"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>96</v>
       </c>
@@ -37042,8 +37039,9 @@
         <v>4.8852986300000005E-4</v>
       </c>
       <c r="I133"/>
+      <c r="K133"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
         <v>96</v>
       </c>
@@ -37069,8 +37067,9 @@
         <v>-6.5795214600000003E-12</v>
       </c>
       <c r="I134"/>
+      <c r="K134"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>96</v>
       </c>
@@ -37096,8 +37095,9 @@
         <v>-0.98972729999999998</v>
       </c>
       <c r="I135"/>
+      <c r="K135"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>96</v>
       </c>
@@ -37123,8 +37123,9 @@
         <v>0.13866529999999999</v>
       </c>
       <c r="I136"/>
+      <c r="K136"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>96</v>
       </c>
@@ -37150,8 +37151,9 @@
         <v>-2.0333689999999999E-4</v>
       </c>
       <c r="I137"/>
+      <c r="K137"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>96</v>
       </c>
@@ -37177,8 +37179,9 @@
         <v>3.3990309999999999E-5</v>
       </c>
       <c r="I138"/>
+      <c r="K138"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>96</v>
       </c>
@@ -37204,8 +37207,9 @@
         <v>-9.5700000000000003E-8</v>
       </c>
       <c r="I139"/>
+      <c r="K139"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
         <v>96</v>
       </c>
@@ -37231,8 +37235,9 @@
         <v>3.2499999999999998E-6</v>
       </c>
       <c r="I140"/>
+      <c r="K140"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141"/>
@@ -37242,8 +37247,9 @@
       <c r="G141" s="14"/>
       <c r="H141"/>
       <c r="I141"/>
+      <c r="K141"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
         <v>97</v>
       </c>
@@ -37269,8 +37275,9 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I142"/>
+      <c r="K142"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>97</v>
       </c>
@@ -37296,8 +37303,9 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I143"/>
+      <c r="K143"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>97</v>
       </c>
@@ -37323,8 +37331,9 @@
         <v>99</v>
       </c>
       <c r="I144"/>
+      <c r="K144"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="B145"/>
       <c r="C145"/>
@@ -37334,8 +37343,9 @@
       <c r="G145" s="14"/>
       <c r="H145"/>
       <c r="I145"/>
+      <c r="K145"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>100</v>
       </c>
@@ -37361,8 +37371,9 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I146"/>
+      <c r="K146"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>100</v>
       </c>
@@ -37388,8 +37399,9 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I147"/>
+      <c r="K147"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>100</v>
       </c>
@@ -37415,8 +37427,9 @@
         <v>101</v>
       </c>
       <c r="I148"/>
+      <c r="K148"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149"/>
       <c r="B149"/>
       <c r="C149"/>
@@ -37426,8 +37439,9 @@
       <c r="G149" s="14"/>
       <c r="H149"/>
       <c r="I149"/>
+      <c r="K149"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>102</v>
       </c>
@@ -37455,8 +37469,9 @@
       <c r="I150" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K150"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>102</v>
       </c>
@@ -37484,8 +37499,9 @@
       <c r="I151" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K151"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
         <v>102</v>
       </c>
@@ -37511,8 +37527,9 @@
         <v>19.987358835277099</v>
       </c>
       <c r="I152"/>
+      <c r="K152"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>102</v>
       </c>
@@ -37538,8 +37555,9 @@
         <v>107</v>
       </c>
       <c r="I153"/>
+      <c r="K153"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>102</v>
       </c>
@@ -37565,8 +37583,9 @@
         <v>109</v>
       </c>
       <c r="I154"/>
+      <c r="K154"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>102</v>
       </c>
@@ -37592,8 +37611,9 @@
         <v>111</v>
       </c>
       <c r="I155"/>
+      <c r="K155"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>102</v>
       </c>
@@ -37619,8 +37639,9 @@
         <v>113</v>
       </c>
       <c r="I156"/>
+      <c r="K156"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157"/>
       <c r="B157"/>
       <c r="C157"/>
@@ -37630,8 +37651,9 @@
       <c r="G157" s="14"/>
       <c r="H157"/>
       <c r="I157"/>
+      <c r="K157"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
         <v>114</v>
       </c>
@@ -37657,8 +37679,9 @@
         <v>117</v>
       </c>
       <c r="I158"/>
+      <c r="K158"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>114</v>
       </c>
@@ -37684,8 +37707,9 @@
         <v>119</v>
       </c>
       <c r="I159"/>
+      <c r="K159"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
         <v>114</v>
       </c>
@@ -37711,8 +37735,9 @@
         <v>121</v>
       </c>
       <c r="I160"/>
+      <c r="K160"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161"/>
       <c r="B161"/>
       <c r="C161"/>
@@ -37722,8 +37747,9 @@
       <c r="G161" s="14"/>
       <c r="H161"/>
       <c r="I161"/>
+      <c r="K161"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>122</v>
       </c>
@@ -37749,8 +37775,9 @@
         <v>25000</v>
       </c>
       <c r="I162"/>
+      <c r="K162"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>122</v>
       </c>
@@ -37776,8 +37803,9 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I163"/>
+      <c r="K163"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>122</v>
       </c>
@@ -37803,8 +37831,9 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I164"/>
+      <c r="K164"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>122</v>
       </c>
@@ -37830,8 +37859,9 @@
         <v>0.45</v>
       </c>
       <c r="I165"/>
+      <c r="K165"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
         <v>122</v>
       </c>
@@ -37857,8 +37887,9 @@
         <v>0.45</v>
       </c>
       <c r="I166"/>
+      <c r="K166"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>122</v>
       </c>
@@ -37884,8 +37915,9 @@
         <v>0.45</v>
       </c>
       <c r="I167"/>
+      <c r="K167"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>122</v>
       </c>
@@ -37911,8 +37943,9 @@
         <v>0.45</v>
       </c>
       <c r="I168"/>
+      <c r="K168"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169"/>
       <c r="B169"/>
       <c r="C169"/>
@@ -37922,8 +37955,9 @@
       <c r="G169" s="14"/>
       <c r="H169"/>
       <c r="I169"/>
+      <c r="K169"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
         <v>128</v>
       </c>
@@ -37949,8 +37983,9 @@
         <v>44.658383333333298</v>
       </c>
       <c r="I170"/>
+      <c r="K170"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>128</v>
       </c>
@@ -37976,8 +38011,9 @@
         <v>-124.095583333333</v>
       </c>
       <c r="I171"/>
+      <c r="K171"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172"/>
       <c r="B172"/>
       <c r="C172"/>
@@ -37987,8 +38023,9 @@
       <c r="G172" s="14"/>
       <c r="H172"/>
       <c r="I172"/>
+      <c r="K172"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>129</v>
       </c>
@@ -38014,8 +38051,9 @@
         <v>601.76969999999994</v>
       </c>
       <c r="I173"/>
+      <c r="K173"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="12" t="s">
         <v>129</v>
       </c>
@@ -38041,8 +38079,9 @@
         <v>4.9606469999999998</v>
       </c>
       <c r="I174"/>
+      <c r="K174"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>129</v>
       </c>
@@ -38068,8 +38107,9 @@
         <v>-1135.396</v>
       </c>
       <c r="I175"/>
+      <c r="K175"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>129</v>
       </c>
@@ -38095,8 +38135,9 @@
         <v>2.6914E-2</v>
       </c>
       <c r="I176"/>
+      <c r="K176"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>129</v>
       </c>
@@ -38122,8 +38163,9 @@
         <v>0</v>
       </c>
       <c r="I177"/>
+      <c r="K177"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>129</v>
       </c>
@@ -38151,8 +38193,9 @@
       <c r="I178" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K178"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>129</v>
       </c>
@@ -38178,8 +38221,9 @@
         <v>0</v>
       </c>
       <c r="I179"/>
+      <c r="K179"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>129</v>
       </c>
@@ -38207,8 +38251,9 @@
       <c r="I180" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="K180"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>129</v>
       </c>
@@ -38234,8 +38279,9 @@
         <v>27.81081</v>
       </c>
       <c r="I181"/>
+      <c r="K181"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>129</v>
       </c>
@@ -38261,8 +38307,9 @@
         <v>0.55913900000000005</v>
       </c>
       <c r="I182"/>
+      <c r="K182"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>129</v>
       </c>
@@ -38288,8 +38335,9 @@
         <v>19.907679999999999</v>
       </c>
       <c r="I183"/>
+      <c r="K183"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
         <v>129</v>
       </c>
@@ -38316,8 +38364,9 @@
       </c>
       <c r="I184"/>
       <c r="J184"/>
+      <c r="K184"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>129</v>
       </c>
@@ -38344,8 +38393,9 @@
       </c>
       <c r="I185"/>
       <c r="J185"/>
+      <c r="K185"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>129</v>
       </c>
@@ -38372,8 +38422,9 @@
       </c>
       <c r="I186"/>
       <c r="J186"/>
+      <c r="K186"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>129</v>
       </c>
@@ -38400,8 +38451,9 @@
       </c>
       <c r="I187"/>
       <c r="J187"/>
+      <c r="K187"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
         <v>129</v>
       </c>
@@ -38427,8 +38479,9 @@
         <v>0</v>
       </c>
       <c r="I188"/>
+      <c r="K188"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>129</v>
       </c>
@@ -38454,8 +38507,9 @@
         <v>8388.6</v>
       </c>
       <c r="I189"/>
+      <c r="K189"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>129</v>
       </c>
@@ -38481,8 +38535,9 @@
         <v>125829.1</v>
       </c>
       <c r="I190"/>
+      <c r="K190"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191"/>
       <c r="B191"/>
       <c r="C191"/>
@@ -38492,8 +38547,9 @@
       <c r="G191" s="14"/>
       <c r="H191"/>
       <c r="I191"/>
+      <c r="K191"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
         <v>148</v>
       </c>
@@ -38519,8 +38575,9 @@
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="I192"/>
+      <c r="K192"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>148</v>
       </c>
@@ -38546,8 +38603,9 @@
         <v>0.76880000000000004</v>
       </c>
       <c r="I193"/>
+      <c r="K193"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
         <v>148</v>
       </c>
@@ -38573,8 +38631,9 @@
         <v>-1.6688000000000001</v>
       </c>
       <c r="I194"/>
+      <c r="K194"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>148</v>
       </c>
@@ -38600,8 +38659,9 @@
         <v>15.7</v>
       </c>
       <c r="I195"/>
+      <c r="K195"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>148</v>
       </c>
@@ -38627,8 +38687,9 @@
         <v>19706</v>
       </c>
       <c r="I196"/>
+      <c r="K196"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>148</v>
       </c>
@@ -38654,8 +38715,9 @@
         <v>34</v>
       </c>
       <c r="I197"/>
+      <c r="K197"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
         <v>148</v>
       </c>
@@ -38681,8 +38743,9 @@
         <v>3073</v>
       </c>
       <c r="I198"/>
+      <c r="K198"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>148</v>
       </c>
@@ -38708,8 +38771,9 @@
         <v>44327</v>
       </c>
       <c r="I199"/>
+      <c r="K199"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200"/>
       <c r="B200"/>
       <c r="C200"/>
@@ -38719,8 +38783,9 @@
       <c r="G200" s="14"/>
       <c r="H200"/>
       <c r="I200"/>
+      <c r="K200"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>156</v>
       </c>
@@ -38746,8 +38811,9 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="I201"/>
+      <c r="K201"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
         <v>156</v>
       </c>
@@ -38773,8 +38839,9 @@
         <v>0.73519999999999996</v>
       </c>
       <c r="I202"/>
+      <c r="K202"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>156</v>
       </c>
@@ -38801,8 +38868,9 @@
       </c>
       <c r="I203"/>
       <c r="J203"/>
+      <c r="K203"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
         <v>156</v>
       </c>
@@ -38829,8 +38897,9 @@
       </c>
       <c r="I204"/>
       <c r="J204"/>
+      <c r="K204"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
         <v>156</v>
       </c>
@@ -38857,8 +38926,9 @@
       </c>
       <c r="I205"/>
       <c r="J205"/>
+      <c r="K205"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
         <v>156</v>
       </c>
@@ -38885,8 +38955,9 @@
       </c>
       <c r="I206"/>
       <c r="J206"/>
+      <c r="K206"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>156</v>
       </c>
@@ -38913,8 +38984,9 @@
       </c>
       <c r="I207"/>
       <c r="J207"/>
+      <c r="K207"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
         <v>156</v>
       </c>
@@ -38940,8 +39012,9 @@
         <v>44327</v>
       </c>
       <c r="I208"/>
+      <c r="K208"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209"/>
       <c r="B209"/>
       <c r="C209"/>
@@ -38950,8 +39023,9 @@
       <c r="F209"/>
       <c r="G209" s="14"/>
       <c r="I209"/>
+      <c r="K209"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210"/>
       <c r="B210"/>
       <c r="C210"/>
@@ -38962,8 +39036,9 @@
       <c r="J210" s="12" t="s">
         <v>158</v>
       </c>
+      <c r="K210"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211"/>
       <c r="B211"/>
       <c r="C211"/>
@@ -38972,8 +39047,9 @@
       <c r="F211"/>
       <c r="G211" s="14"/>
       <c r="J211"/>
+      <c r="K211"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212"/>
       <c r="B212"/>
       <c r="C212"/>
@@ -38984,8 +39060,9 @@
       <c r="J212" s="12" t="s">
         <v>159</v>
       </c>
+      <c r="K212"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213"/>
       <c r="B213"/>
       <c r="C213"/>
@@ -38994,8 +39071,9 @@
       <c r="F213"/>
       <c r="G213" s="14"/>
       <c r="I213"/>
+      <c r="K213"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
         <v>160</v>
       </c>
@@ -39018,8 +39096,9 @@
       <c r="I214" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K214"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>162</v>
       </c>
@@ -39042,8 +39121,9 @@
       <c r="I215" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K215"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216"/>
       <c r="B216"/>
       <c r="C216"/>
@@ -39052,8 +39132,9 @@
       <c r="F216" s="18"/>
       <c r="G216" s="14"/>
       <c r="I216"/>
+      <c r="K216"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
         <v>164</v>
       </c>
@@ -39076,8 +39157,9 @@
       <c r="I217" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K217"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
         <v>166</v>
       </c>
@@ -39100,8 +39182,9 @@
       <c r="I218" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K218"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>168</v>
       </c>
@@ -39123,8 +39206,9 @@
       <c r="I219" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K219"/>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>170</v>
       </c>
@@ -39146,6 +39230,7 @@
       <c r="I220" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K220"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>